<commit_message>
Computed median iterations in benders results.
</commit_message>
<xml_diff>
--- a/results/storm_j10/benders_results_j10.xlsx
+++ b/results/storm_j10/benders_results_j10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="benders_results_0" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2848" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="558">
   <si>
     <t xml:space="preserve">instance</t>
   </si>
@@ -1646,13 +1646,10 @@
     <t xml:space="preserve">j1064_3</t>
   </si>
   <si>
-    <t xml:space="preserve">j1064_4</t>
-  </si>
-  <si>
     <t xml:space="preserve">total solved</t>
   </si>
   <si>
-    <t xml:space="preserve">j1064_5</t>
+    <t xml:space="preserve">j1064_4</t>
   </si>
   <si>
     <t xml:space="preserve">avg. gap</t>
@@ -1661,19 +1658,25 @@
     <t xml:space="preserve">(excl. instances where no feasible solution was found)</t>
   </si>
   <si>
-    <t xml:space="preserve">j1064_6</t>
+    <t xml:space="preserve">j1064_5</t>
   </si>
   <si>
     <t xml:space="preserve">avg. non-opt gap</t>
   </si>
   <si>
-    <t xml:space="preserve">j1064_7</t>
+    <t xml:space="preserve">j1064_6</t>
   </si>
   <si>
     <t xml:space="preserve">avg. iterations</t>
   </si>
   <si>
     <t xml:space="preserve">(excl. iterations that weren’t completed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j1064_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">median iterations</t>
   </si>
   <si>
     <t xml:space="preserve">j1064_8</t>
@@ -1709,6 +1712,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1768,12 +1772,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1796,8 +1804,8 @@
   </sheetPr>
   <dimension ref="A1:L537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A496" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L537" activeCellId="0" sqref="L537"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A506" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J530" activeCellId="0" sqref="J530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15594,10 +15602,17 @@
       <c r="H530" s="0" t="n">
         <v>0.837</v>
       </c>
+      <c r="J530" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="K530" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E537,0)</f>
+        <v>533</v>
+      </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>0</v>
@@ -15621,16 +15636,19 @@
         <v>0.465</v>
       </c>
       <c r="J531" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="K531" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E537,0)</f>
-        <v>533</v>
+        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
+        <v>0</v>
+      </c>
+      <c r="L531" s="0" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>0</v>
@@ -15654,19 +15672,19 @@
         <v>1.513</v>
       </c>
       <c r="J532" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="K532" s="0" t="e">
+        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L532" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="K532" s="0" t="n">
-        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
-        <v>0</v>
-      </c>
-      <c r="L532" s="0" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>0</v>
@@ -15690,19 +15708,19 @@
         <v>0.621</v>
       </c>
       <c r="J533" s="0" t="s">
-        <v>546</v>
-      </c>
-      <c r="K533" s="0" t="e">
-        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L533" s="1" t="s">
-        <v>544</v>
+        <v>547</v>
+      </c>
+      <c r="K533" s="0" t="n">
+        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="L533" s="0" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>0</v>
@@ -15726,19 +15744,19 @@
         <v>1.183</v>
       </c>
       <c r="J534" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="K534" s="2" t="n">
+        <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
+        <v>1</v>
+      </c>
+      <c r="L534" s="0" t="s">
         <v>548</v>
-      </c>
-      <c r="K534" s="0" t="n">
-        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
-        <v>1</v>
-      </c>
-      <c r="L534" s="0" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>0</v>
@@ -15762,19 +15780,19 @@
         <v>0.468</v>
       </c>
       <c r="J535" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="K535" s="0" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>59.5076941838649</v>
       </c>
       <c r="L535" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>0</v>
@@ -15798,19 +15816,19 @@
         <v>0.671</v>
       </c>
       <c r="J536" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="K536" s="0" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>79.5115447761194</v>
       </c>
       <c r="L536" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>0</v>
@@ -15834,7 +15852,7 @@
         <v>0.819</v>
       </c>
       <c r="J537" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="K537" s="0" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;&gt;*3600")</f>
@@ -15859,8 +15877,8 @@
   </sheetPr>
   <dimension ref="A1:L537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A503" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L537" activeCellId="0" sqref="L537"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A502" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J530" activeCellId="0" sqref="J530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15874,7 +15892,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.94"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -29657,10 +29675,17 @@
       <c r="H530" s="0" t="n">
         <v>36.72</v>
       </c>
+      <c r="J530" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="K530" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E537,0)</f>
+        <v>388</v>
+      </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>3</v>
@@ -29684,16 +29709,19 @@
         <v>3.225</v>
       </c>
       <c r="J531" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="K531" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E537,0)</f>
-        <v>388</v>
+        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
+        <v>0.0587485928705441</v>
+      </c>
+      <c r="L531" s="0" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>3</v>
@@ -29717,19 +29745,19 @@
         <v>83.331</v>
       </c>
       <c r="J532" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="K532" s="0" t="n">
+        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
+        <v>0.215951724137931</v>
+      </c>
+      <c r="L532" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="K532" s="0" t="n">
-        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
-        <v>0.0587485928705441</v>
-      </c>
-      <c r="L532" s="0" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>3</v>
@@ -29753,19 +29781,19 @@
         <v>16.086</v>
       </c>
       <c r="J533" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="K533" s="0" t="n">
-        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
-        <v>0.215951724137931</v>
-      </c>
-      <c r="L533" s="1" t="s">
-        <v>544</v>
+        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
+        <v>67.0863039399625</v>
+      </c>
+      <c r="L533" s="0" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>3</v>
@@ -29789,19 +29817,19 @@
         <v>17.804</v>
       </c>
       <c r="J534" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="K534" s="2" t="n">
+        <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
+        <v>44</v>
+      </c>
+      <c r="L534" s="0" t="s">
         <v>548</v>
-      </c>
-      <c r="K534" s="0" t="n">
-        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
-        <v>67.0863039399625</v>
-      </c>
-      <c r="L534" s="0" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>3</v>
@@ -29825,19 +29853,19 @@
         <v>8.602</v>
       </c>
       <c r="J535" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="K535" s="0" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>53.2679343339587</v>
       </c>
       <c r="L535" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>3</v>
@@ -29861,19 +29889,19 @@
         <v>16.607</v>
       </c>
       <c r="J536" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="K536" s="0" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>1158.96043656717</v>
       </c>
       <c r="L536" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>3</v>
@@ -29897,7 +29925,7 @@
         <v>45.453</v>
       </c>
       <c r="J537" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="K537" s="0" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;&gt;*3600")</f>
@@ -29907,7 +29935,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -29922,8 +29950,8 @@
   </sheetPr>
   <dimension ref="A1:L537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A521" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L537" activeCellId="0" sqref="L537"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B502" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J530" activeCellId="0" sqref="J530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43718,10 +43746,17 @@
       <c r="H530" s="0" t="n">
         <v>75.272</v>
       </c>
+      <c r="J530" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="K530" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E537,0)</f>
+        <v>367</v>
+      </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>5</v>
@@ -43745,16 +43780,19 @@
         <v>5.495</v>
       </c>
       <c r="J531" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="K531" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E537,0)</f>
-        <v>367</v>
+        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
+        <v>0.0765996240601503</v>
+      </c>
+      <c r="L531" s="0" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>5</v>
@@ -43778,19 +43816,19 @@
         <v>162.23</v>
       </c>
       <c r="J532" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="K532" s="0" t="n">
+        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
+        <v>0.246975757575757</v>
+      </c>
+      <c r="L532" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="K532" s="0" t="n">
-        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
-        <v>0.0765996240601503</v>
-      </c>
-      <c r="L532" s="0" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>5</v>
@@ -43814,19 +43852,19 @@
         <v>25.695</v>
       </c>
       <c r="J533" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="K533" s="0" t="n">
-        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
-        <v>0.246975757575757</v>
-      </c>
-      <c r="L533" s="1" t="s">
-        <v>544</v>
+        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
+        <v>67.6146616541353</v>
+      </c>
+      <c r="L533" s="0" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>5</v>
@@ -43850,19 +43888,19 @@
         <v>31.556</v>
       </c>
       <c r="J534" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="K534" s="2" t="n">
+        <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
+        <v>46</v>
+      </c>
+      <c r="L534" s="0" t="s">
         <v>548</v>
-      </c>
-      <c r="K534" s="0" t="n">
-        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
-        <v>67.6146616541353</v>
-      </c>
-      <c r="L534" s="0" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>5</v>
@@ -43886,19 +43924,19 @@
         <v>14.957</v>
       </c>
       <c r="J535" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="K535" s="0" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>71.6395432330828</v>
       </c>
       <c r="L535" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>5</v>
@@ -43922,19 +43960,19 @@
         <v>30.654</v>
       </c>
       <c r="J536" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="K536" s="0" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>1313.4033358209</v>
       </c>
       <c r="L536" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>5</v>
@@ -43958,7 +43996,7 @@
         <v>84.53</v>
       </c>
       <c r="J537" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="K537" s="0" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;&gt;*3600")</f>
@@ -43968,7 +44006,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -43984,7 +44022,7 @@
   <dimension ref="A1:L537"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A505" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M529" activeCellId="0" sqref="M529"/>
+      <selection pane="topLeft" activeCell="J530" activeCellId="0" sqref="J530"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -57779,10 +57817,17 @@
       <c r="H530" s="0" t="n">
         <v>63.544</v>
       </c>
+      <c r="J530" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="K530" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E537,0)</f>
+        <v>373</v>
+      </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>7</v>
@@ -57806,16 +57851,19 @@
         <v>4.406</v>
       </c>
       <c r="J531" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="K531" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E537,0)</f>
-        <v>373</v>
+        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
+        <v>0.075375234521576</v>
+      </c>
+      <c r="L531" s="0" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>7</v>
@@ -57839,19 +57887,19 @@
         <v>122.734</v>
       </c>
       <c r="J532" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="K532" s="0" t="n">
+        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
+        <v>0.25109375</v>
+      </c>
+      <c r="L532" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="K532" s="0" t="n">
-        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
-        <v>0.075375234521576</v>
-      </c>
-      <c r="L532" s="0" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>7</v>
@@ -57875,19 +57923,19 @@
         <v>24.257</v>
       </c>
       <c r="J533" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="K533" s="0" t="n">
-        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
-        <v>0.25109375</v>
-      </c>
-      <c r="L533" s="1" t="s">
-        <v>544</v>
+        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
+        <v>73.703564727955</v>
+      </c>
+      <c r="L533" s="0" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>7</v>
@@ -57911,19 +57959,19 @@
         <v>18.071</v>
       </c>
       <c r="J534" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="K534" s="2" t="n">
+        <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
+        <v>49.5</v>
+      </c>
+      <c r="L534" s="0" t="s">
         <v>548</v>
-      </c>
-      <c r="K534" s="0" t="n">
-        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
-        <v>73.703564727955</v>
-      </c>
-      <c r="L534" s="0" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>7</v>
@@ -57947,19 +57995,19 @@
         <v>9.848</v>
       </c>
       <c r="J535" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="K535" s="0" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>56.4673621013133</v>
       </c>
       <c r="L535" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>7</v>
@@ -57983,19 +58031,19 @@
         <v>20.24</v>
       </c>
       <c r="J536" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="K536" s="0" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>1261.47342350746</v>
       </c>
       <c r="L536" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>7</v>
@@ -58019,7 +58067,7 @@
         <v>54.466</v>
       </c>
       <c r="J537" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="K537" s="0" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;3600")</f>
@@ -58029,7 +58077,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -58044,8 +58092,8 @@
   </sheetPr>
   <dimension ref="A1:L537"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A503" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L537" activeCellId="0" sqref="L537"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A501" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J543" activeCellId="0" sqref="J543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -71842,10 +71890,17 @@
       <c r="H530" s="0" t="n">
         <v>90.471</v>
       </c>
+      <c r="J530" s="0" t="s">
+        <v>540</v>
+      </c>
+      <c r="K530" s="0" t="n">
+        <f aca="false">COUNTIF(E2:E537,0)</f>
+        <v>368</v>
+      </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B531" s="0" t="n">
         <v>10</v>
@@ -71869,16 +71924,19 @@
         <v>5.882</v>
       </c>
       <c r="J531" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="K531" s="0" t="n">
-        <f aca="false">COUNTIF(E2:E537,0)</f>
-        <v>368</v>
+        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
+        <v>0.0787011278195489</v>
+      </c>
+      <c r="L531" s="0" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B532" s="0" t="n">
         <v>10</v>
@@ -71902,19 +71960,19 @@
         <v>152.943</v>
       </c>
       <c r="J532" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="K532" s="0" t="n">
+        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
+        <v>0.255298780487805</v>
+      </c>
+      <c r="L532" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="K532" s="0" t="n">
-        <f aca="false">AVERAGEIF(E2:E537,"&lt;&gt;*nan")</f>
-        <v>0.0787011278195489</v>
-      </c>
-      <c r="L532" s="0" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B533" s="0" t="n">
         <v>10</v>
@@ -71938,19 +71996,19 @@
         <v>19.815</v>
       </c>
       <c r="J533" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="K533" s="0" t="n">
-        <f aca="false">AVERAGEIFS(E2:E537,E2:E537,"&lt;&gt;*nan",E2:E537,"&lt;&gt;0")</f>
-        <v>0.255298780487805</v>
-      </c>
-      <c r="L533" s="1" t="s">
-        <v>544</v>
+        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
+        <v>68.812030075188</v>
+      </c>
+      <c r="L533" s="0" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B534" s="0" t="n">
         <v>10</v>
@@ -71974,19 +72032,19 @@
         <v>31.581</v>
       </c>
       <c r="J534" s="0" t="s">
+        <v>550</v>
+      </c>
+      <c r="K534" s="2" t="n">
+        <f aca="false">MEDIAN(IF(F2:F537&lt;&gt;0,F2:F537))</f>
+        <v>46</v>
+      </c>
+      <c r="L534" s="0" t="s">
         <v>548</v>
-      </c>
-      <c r="K534" s="0" t="n">
-        <f aca="false">AVERAGEIF(F2:F537,"&lt;&gt;0")</f>
-        <v>68.812030075188</v>
-      </c>
-      <c r="L534" s="0" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B535" s="0" t="n">
         <v>10</v>
@@ -72010,19 +72068,19 @@
         <v>15.495</v>
       </c>
       <c r="J535" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="K535" s="0" t="n">
         <f aca="false">AVERAGEIF(G2:G537,"&lt;&gt;*inf")</f>
         <v>70.7793646616541</v>
       </c>
       <c r="L535" s="0" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B536" s="0" t="n">
         <v>10</v>
@@ -72046,19 +72104,19 @@
         <v>35.209</v>
       </c>
       <c r="J536" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="K536" s="0" t="n">
         <f aca="false">AVERAGE(H2:H537)</f>
         <v>1317.23424067164</v>
       </c>
       <c r="L536" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B537" s="0" t="n">
         <v>10</v>
@@ -72082,7 +72140,7 @@
         <v>76.554</v>
       </c>
       <c r="J537" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="K537" s="0" t="n">
         <f aca="false">AVERAGEIF(H2:H537,"&lt;&gt;*3600")</f>
@@ -72092,7 +72150,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>